<commit_message>
add complete salary table
</commit_message>
<xml_diff>
--- a/Data/PA-PSERS.xlsx
+++ b/Data/PA-PSERS.xlsx
@@ -394,7 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -5063,7 +5063,7 @@
   <dimension ref="A3:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5081,7 +5081,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="11">
-        <v>0.1075</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>